<commit_message>
En første løsing av oppgave 1 er implementert i Pyomo.
</commit_message>
<xml_diff>
--- a/exercise-6/Produkt_miks.xlsx
+++ b/exercise-6/Produkt_miks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Basismodell" sheetId="1" state="visible" r:id="rId2"/>
@@ -664,8 +664,8 @@
   </sheetPr>
   <dimension ref="B1:K30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H43" activeCellId="0" sqref="H43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -872,7 +872,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P25" activeCellId="0" sqref="P25"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1074,7 +1074,7 @@
   </sheetPr>
   <dimension ref="A1:AA44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="R36" activeCellId="0" sqref="R36"/>
     </sheetView>
   </sheetViews>
@@ -1894,7 +1894,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Nytt navn på et par filer og skrevet funksjonalitet for å fylle inn løsingen i Excel-filen.
</commit_message>
<xml_diff>
--- a/exercise-6/Produkt_miks.xlsx
+++ b/exercise-6/Produkt_miks.xlsx
@@ -254,7 +254,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">Løst i Python:</t>
+  </si>
   <si>
     <t xml:space="preserve">Legering</t>
   </si>
@@ -322,7 +325,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -355,20 +358,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFFF2CC"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF202124"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,6 +379,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF5983B0"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6D6D"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFDAE3F3"/>
         <bgColor rgb="FFE2F0D9"/>
       </patternFill>
@@ -393,75 +401,13 @@
         <bgColor rgb="FFE2F0D9"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC0B699"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -488,20 +434,18 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -509,79 +453,31 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="6" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="7" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,14 +506,14 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0B699"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFF2CC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF6D6D"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFDAE3F3"/>
       <rgbColor rgb="FF000080"/>
@@ -642,7 +538,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF5983B0"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -665,23 +561,26 @@
   <dimension ref="B1:K30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.31"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="2" t="n">
         <v>606035</v>
       </c>
@@ -695,16 +594,16 @@
         <v>606017</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K3" s="4" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0.15</v>
@@ -719,140 +618,180 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="n">
         <v>152</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9" t="n">
+      <c r="D5" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6" t="n">
         <f aca="false">SUM(D5:G5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="n">
         <v>178</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>0.13</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="9" t="n">
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6" t="n">
         <f aca="false">SUM(D6:G6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="n">
         <v>203</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>0.05</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="9" t="n">
+      <c r="D7" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6" t="n">
         <f aca="false">SUM(D7:G7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
         <v>215</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>0.26</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="9" t="n">
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="H8" s="6" t="n">
         <f aca="false">SUM(D8:G8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="n">
         <v>254</v>
       </c>
       <c r="C9" s="5" t="n">
         <v>0.06</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="9" t="n">
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6" t="n">
         <f aca="false">SUM(D9:G9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="9" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D10" s="6" t="n">
         <f aca="false">SUM(D5:D9)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="9" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="E10" s="6" t="n">
         <f aca="false">SUM(E5:E9)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="9" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="F10" s="6" t="n">
         <f aca="false">SUM(F5:F9)</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="9" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="G10" s="6" t="n">
         <f aca="false">SUM(G5:G9)</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="16"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="17"/>
+        <v>0.16</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="7"/>
       <c r="C14" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="18"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="8"/>
       <c r="C15" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="4"/>
       <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -875,24 +814,23 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="D3" s="2" t="n">
         <v>606035</v>
@@ -907,155 +845,150 @@
         <v>606017</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K3" s="4" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="1" t="n">
         <v>0.24</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="1" t="n">
         <v>0.45</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="1" t="n">
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9" t="n">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="n">
         <f aca="false">SUM(D5:G5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="n">
         <v>178</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="1" t="n">
         <v>0.13</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="9" t="n">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="n">
         <f aca="false">SUM(D6:G6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="n">
         <v>203</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="9" t="n">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="n">
         <f aca="false">SUM(D7:G7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
         <v>215</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="1" t="n">
         <v>0.26</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="9" t="n">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="n">
         <f aca="false">SUM(D8:G8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="n">
         <v>254</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="1" t="n">
         <v>0.06</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="9" t="n">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="n">
         <f aca="false">SUM(D9:G9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="9" t="n">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D10" s="1" t="n">
         <f aca="false">SUM(D5:D9)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="9" t="n">
+      <c r="E10" s="1" t="n">
         <f aca="false">SUM(E5:E9)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="9" t="n">
+      <c r="F10" s="1" t="n">
         <f aca="false">SUM(F5:F9)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="9" t="n">
+      <c r="G10" s="1" t="n">
         <f aca="false">SUM(G5:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="16"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="17"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="7"/>
       <c r="C14" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="18"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="8"/>
       <c r="C15" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="4"/>
       <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1078,25 +1011,22 @@
       <selection pane="topLeft" activeCell="R36" activeCellId="0" sqref="R36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.42"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="2" t="n">
         <v>606035</v>
       </c>
@@ -1110,183 +1040,178 @@
         <v>606017</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K4" s="4" t="n">
         <f aca="false">SUM(L17:O21)+SUM(R17:U21)</f>
         <v>0.9985</v>
       </c>
-      <c r="O4" s="17"/>
+      <c r="O4" s="7"/>
       <c r="P4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="1" t="n">
         <v>0.24</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="1" t="n">
         <v>0.45</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="O5" s="18"/>
+      <c r="O5" s="8"/>
       <c r="P5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9" t="n">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="n">
         <f aca="false">SUM(D6:G6)</f>
         <v>0</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="n">
         <v>178</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="1" t="n">
         <v>0.13</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="9" t="n">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="n">
         <f aca="false">SUM(D7:G7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
         <v>203</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="9" t="n">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="n">
         <f aca="false">SUM(D8:G8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="n">
         <v>215</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="1" t="n">
         <v>0.26</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="9" t="n">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="n">
         <f aca="false">SUM(D9:G9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="n">
         <v>254</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="1" t="n">
         <v>0.06</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="9" t="n">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="n">
         <f aca="false">SUM(D10:G10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="9" t="n">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D11" s="1" t="n">
         <f aca="false">SUM(D6:D10)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="9" t="n">
+      <c r="E11" s="1" t="n">
         <f aca="false">SUM(E6:E10)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="9" t="n">
+      <c r="F11" s="1" t="n">
         <f aca="false">SUM(F6:F10)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="9" t="n">
+      <c r="G11" s="1" t="n">
         <f aca="false">SUM(G6:G10)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="16"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="L13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>606035</v>
@@ -1301,10 +1226,10 @@
         <v>606017</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L16" s="2" t="n">
         <v>606035</v>
@@ -1319,7 +1244,7 @@
         <v>606017</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R16" s="2" t="n">
         <v>606035</v>
@@ -1334,7 +1259,7 @@
         <v>606017</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X16" s="2" t="n">
         <v>606035</v>
@@ -1349,395 +1274,395 @@
         <v>606017</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="s">
-        <v>14</v>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="D17" s="1" t="n">
         <v>0.093</v>
       </c>
-      <c r="E17" s="5" t="n">
+      <c r="E17" s="1" t="n">
         <v>0.085</v>
       </c>
-      <c r="F17" s="5" t="n">
+      <c r="F17" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="G17" s="5" t="n">
+      <c r="G17" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="I17" s="22" t="n">
+      <c r="I17" s="10" t="n">
         <f aca="false">SUM(D17:G21)</f>
         <v>0.9985</v>
       </c>
       <c r="K17" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="L17" s="11" t="n">
+      <c r="L17" s="1" t="n">
         <f aca="false">MAX(0, D25)</f>
         <v>0</v>
       </c>
-      <c r="M17" s="11" t="n">
+      <c r="M17" s="1" t="n">
         <f aca="false">MAX(0, E25)</f>
         <v>0</v>
       </c>
-      <c r="N17" s="11" t="n">
+      <c r="N17" s="1" t="n">
         <f aca="false">MAX(0, F25)</f>
         <v>0</v>
       </c>
-      <c r="O17" s="11" t="n">
+      <c r="O17" s="1" t="n">
         <f aca="false">MAX(0, G25)</f>
         <v>0</v>
       </c>
       <c r="Q17" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="R17" s="11" t="n">
+      <c r="R17" s="1" t="n">
         <f aca="false">-MIN(0, D25)</f>
         <v>0.093</v>
       </c>
-      <c r="S17" s="11" t="n">
+      <c r="S17" s="1" t="n">
         <f aca="false">-MIN(0, E25)</f>
         <v>0.085</v>
       </c>
-      <c r="T17" s="11" t="n">
+      <c r="T17" s="1" t="n">
         <f aca="false">-MIN(0, F25)</f>
         <v>0.25</v>
       </c>
-      <c r="U17" s="11" t="n">
+      <c r="U17" s="1" t="n">
         <f aca="false">-MIN(0, G25)</f>
         <v>0.02</v>
       </c>
       <c r="W17" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="X17" s="9" t="n">
+      <c r="X17" s="1" t="n">
         <f aca="false">L17-R17</f>
         <v>-0.093</v>
       </c>
-      <c r="Y17" s="9" t="n">
+      <c r="Y17" s="1" t="n">
         <f aca="false">M17-S17</f>
         <v>-0.085</v>
       </c>
-      <c r="Z17" s="9" t="n">
+      <c r="Z17" s="1" t="n">
         <f aca="false">N17-T17</f>
         <v>-0.25</v>
       </c>
-      <c r="AA17" s="9" t="n">
+      <c r="AA17" s="1" t="n">
         <f aca="false">O17-U17</f>
         <v>-0.02</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C18" s="2" t="n">
         <v>178</v>
       </c>
-      <c r="D18" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5" t="n">
+      <c r="D18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="F18" s="5" t="n">
+      <c r="F18" s="1" t="n">
         <v>0.0005</v>
       </c>
-      <c r="G18" s="5" t="n">
+      <c r="G18" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="K18" s="2" t="n">
         <v>178</v>
       </c>
-      <c r="L18" s="11" t="n">
+      <c r="L18" s="1" t="n">
         <f aca="false">MAX(0, D26)</f>
         <v>0</v>
       </c>
-      <c r="M18" s="11" t="n">
+      <c r="M18" s="1" t="n">
         <f aca="false">MAX(0, E26)</f>
         <v>0</v>
       </c>
-      <c r="N18" s="11" t="n">
+      <c r="N18" s="1" t="n">
         <f aca="false">MAX(0, F26)</f>
         <v>0</v>
       </c>
-      <c r="O18" s="11" t="n">
+      <c r="O18" s="1" t="n">
         <f aca="false">MAX(0, G26)</f>
         <v>0</v>
       </c>
       <c r="Q18" s="2" t="n">
         <v>178</v>
       </c>
-      <c r="R18" s="11" t="n">
+      <c r="R18" s="1" t="n">
         <f aca="false">-MIN(0, D26)</f>
         <v>-0</v>
       </c>
-      <c r="S18" s="11" t="n">
+      <c r="S18" s="1" t="n">
         <f aca="false">-MIN(0, E26)</f>
         <v>0.16</v>
       </c>
-      <c r="T18" s="11" t="n">
+      <c r="T18" s="1" t="n">
         <f aca="false">-MIN(0, F26)</f>
         <v>0.0005</v>
       </c>
-      <c r="U18" s="11" t="n">
+      <c r="U18" s="1" t="n">
         <f aca="false">-MIN(0, G26)</f>
         <v>0.01</v>
       </c>
       <c r="W18" s="2" t="n">
         <v>178</v>
       </c>
-      <c r="X18" s="9" t="n">
+      <c r="X18" s="1" t="n">
         <f aca="false">L18-R18</f>
         <v>0</v>
       </c>
-      <c r="Y18" s="9" t="n">
+      <c r="Y18" s="1" t="n">
         <f aca="false">M18-S18</f>
         <v>-0.16</v>
       </c>
-      <c r="Z18" s="9" t="n">
+      <c r="Z18" s="1" t="n">
         <f aca="false">N18-T18</f>
         <v>-0.0005</v>
       </c>
-      <c r="AA18" s="9" t="n">
+      <c r="AA18" s="1" t="n">
         <f aca="false">O18-U18</f>
         <v>-0.01</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C19" s="2" t="n">
         <v>203</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="D19" s="1" t="n">
         <v>0.07</v>
       </c>
-      <c r="E19" s="5" t="n">
+      <c r="E19" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="F19" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="5" t="n">
+      <c r="F19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="2" t="n">
         <v>203</v>
       </c>
-      <c r="L19" s="11" t="n">
+      <c r="L19" s="1" t="n">
         <f aca="false">MAX(0, D27)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="11" t="n">
+      <c r="M19" s="1" t="n">
         <f aca="false">MAX(0, E27)</f>
         <v>0</v>
       </c>
-      <c r="N19" s="11" t="n">
+      <c r="N19" s="1" t="n">
         <f aca="false">MAX(0, F27)</f>
         <v>0</v>
       </c>
-      <c r="O19" s="11" t="n">
+      <c r="O19" s="1" t="n">
         <f aca="false">MAX(0, G27)</f>
         <v>0</v>
       </c>
       <c r="Q19" s="2" t="n">
         <v>203</v>
       </c>
-      <c r="R19" s="11" t="n">
+      <c r="R19" s="1" t="n">
         <f aca="false">-MIN(0, D27)</f>
         <v>0.07</v>
       </c>
-      <c r="S19" s="11" t="n">
+      <c r="S19" s="1" t="n">
         <f aca="false">-MIN(0, E27)</f>
         <v>0.01</v>
       </c>
-      <c r="T19" s="11" t="n">
+      <c r="T19" s="1" t="n">
         <f aca="false">-MIN(0, F27)</f>
         <v>-0</v>
       </c>
-      <c r="U19" s="11" t="n">
+      <c r="U19" s="1" t="n">
         <f aca="false">-MIN(0, G27)</f>
         <v>-0</v>
       </c>
       <c r="W19" s="2" t="n">
         <v>203</v>
       </c>
-      <c r="X19" s="9" t="n">
+      <c r="X19" s="1" t="n">
         <f aca="false">L19-R19</f>
         <v>-0.07</v>
       </c>
-      <c r="Y19" s="9" t="n">
+      <c r="Y19" s="1" t="n">
         <f aca="false">M19-S19</f>
         <v>-0.01</v>
       </c>
-      <c r="Z19" s="9" t="n">
+      <c r="Z19" s="1" t="n">
         <f aca="false">N19-T19</f>
         <v>0</v>
       </c>
-      <c r="AA19" s="9" t="n">
+      <c r="AA19" s="1" t="n">
         <f aca="false">O19-U19</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C20" s="2" t="n">
         <v>215</v>
       </c>
-      <c r="D20" s="5" t="n">
+      <c r="D20" s="1" t="n">
         <v>0.13</v>
       </c>
-      <c r="E20" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="5" t="n">
+      <c r="E20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="n">
         <v>0.11</v>
       </c>
       <c r="K20" s="2" t="n">
         <v>215</v>
       </c>
-      <c r="L20" s="11" t="n">
+      <c r="L20" s="1" t="n">
         <f aca="false">MAX(0, D28)</f>
         <v>0</v>
       </c>
-      <c r="M20" s="11" t="n">
+      <c r="M20" s="1" t="n">
         <f aca="false">MAX(0, E28)</f>
         <v>0</v>
       </c>
-      <c r="N20" s="11" t="n">
+      <c r="N20" s="1" t="n">
         <f aca="false">MAX(0, F28)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="11" t="n">
+      <c r="O20" s="1" t="n">
         <f aca="false">MAX(0, G28)</f>
         <v>0</v>
       </c>
       <c r="Q20" s="2" t="n">
         <v>215</v>
       </c>
-      <c r="R20" s="11" t="n">
+      <c r="R20" s="1" t="n">
         <f aca="false">-MIN(0, D28)</f>
         <v>0.13</v>
       </c>
-      <c r="S20" s="11" t="n">
+      <c r="S20" s="1" t="n">
         <f aca="false">-MIN(0, E28)</f>
         <v>-0</v>
       </c>
-      <c r="T20" s="11" t="n">
+      <c r="T20" s="1" t="n">
         <f aca="false">-MIN(0, F28)</f>
         <v>-0</v>
       </c>
-      <c r="U20" s="11" t="n">
+      <c r="U20" s="1" t="n">
         <f aca="false">-MIN(0, G28)</f>
         <v>0.11</v>
       </c>
       <c r="W20" s="2" t="n">
         <v>215</v>
       </c>
-      <c r="X20" s="9" t="n">
+      <c r="X20" s="1" t="n">
         <f aca="false">L20-R20</f>
         <v>-0.13</v>
       </c>
-      <c r="Y20" s="9" t="n">
+      <c r="Y20" s="1" t="n">
         <f aca="false">M20-S20</f>
         <v>0</v>
       </c>
-      <c r="Z20" s="9" t="n">
+      <c r="Z20" s="1" t="n">
         <f aca="false">N20-T20</f>
         <v>0</v>
       </c>
-      <c r="AA20" s="9" t="n">
+      <c r="AA20" s="1" t="n">
         <f aca="false">O20-U20</f>
         <v>-0.11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C21" s="2" t="n">
         <v>254</v>
       </c>
-      <c r="D21" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="5" t="n">
+      <c r="D21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="F21" s="5" t="n">
+      <c r="F21" s="1" t="n">
         <v>0.03</v>
       </c>
-      <c r="G21" s="5" t="n">
+      <c r="G21" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="K21" s="2" t="n">
         <v>254</v>
       </c>
-      <c r="L21" s="11" t="n">
+      <c r="L21" s="1" t="n">
         <f aca="false">MAX(0, D29)</f>
         <v>0</v>
       </c>
-      <c r="M21" s="11" t="n">
+      <c r="M21" s="1" t="n">
         <f aca="false">MAX(0, E29)</f>
         <v>0</v>
       </c>
-      <c r="N21" s="11" t="n">
+      <c r="N21" s="1" t="n">
         <f aca="false">MAX(0, F29)</f>
         <v>0</v>
       </c>
-      <c r="O21" s="11" t="n">
+      <c r="O21" s="1" t="n">
         <f aca="false">MAX(0, G29)</f>
         <v>0</v>
       </c>
       <c r="Q21" s="2" t="n">
         <v>254</v>
       </c>
-      <c r="R21" s="11" t="n">
+      <c r="R21" s="1" t="n">
         <f aca="false">-MIN(0, D29)</f>
         <v>-0</v>
       </c>
-      <c r="S21" s="11" t="n">
+      <c r="S21" s="1" t="n">
         <f aca="false">-MIN(0, E29)</f>
         <v>0.02</v>
       </c>
-      <c r="T21" s="11" t="n">
+      <c r="T21" s="1" t="n">
         <f aca="false">-MIN(0, F29)</f>
         <v>0.03</v>
       </c>
-      <c r="U21" s="11" t="n">
+      <c r="U21" s="1" t="n">
         <f aca="false">-MIN(0, G29)</f>
         <v>0.01</v>
       </c>
       <c r="W21" s="2" t="n">
         <v>254</v>
       </c>
-      <c r="X21" s="9" t="n">
+      <c r="X21" s="1" t="n">
         <f aca="false">L21-R21</f>
         <v>0</v>
       </c>
-      <c r="Y21" s="9" t="n">
+      <c r="Y21" s="1" t="n">
         <f aca="false">M21-S21</f>
         <v>-0.02</v>
       </c>
-      <c r="Z21" s="9" t="n">
+      <c r="Z21" s="1" t="n">
         <f aca="false">N21-T21</f>
         <v>-0.03</v>
       </c>
-      <c r="AA21" s="9" t="n">
+      <c r="AA21" s="1" t="n">
         <f aca="false">O21-U21</f>
         <v>-0.01</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D23" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24" s="2" t="n">
         <v>606035</v>
@@ -1752,129 +1677,129 @@
         <v>606017</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="D25" s="9" t="n">
+      <c r="D25" s="1" t="n">
         <f aca="false">D6-D17</f>
         <v>-0.093</v>
       </c>
-      <c r="E25" s="9" t="n">
+      <c r="E25" s="1" t="n">
         <f aca="false">E6-E17</f>
         <v>-0.085</v>
       </c>
-      <c r="F25" s="9" t="n">
+      <c r="F25" s="1" t="n">
         <f aca="false">F6-F17</f>
         <v>-0.25</v>
       </c>
-      <c r="G25" s="9" t="n">
+      <c r="G25" s="1" t="n">
         <f aca="false">G6-G17</f>
         <v>-0.02</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C26" s="2" t="n">
         <v>178</v>
       </c>
-      <c r="D26" s="9" t="n">
+      <c r="D26" s="1" t="n">
         <f aca="false">D7-D18</f>
         <v>0</v>
       </c>
-      <c r="E26" s="9" t="n">
+      <c r="E26" s="1" t="n">
         <f aca="false">E7-E18</f>
         <v>-0.16</v>
       </c>
-      <c r="F26" s="9" t="n">
+      <c r="F26" s="1" t="n">
         <f aca="false">F7-F18</f>
         <v>-0.0005</v>
       </c>
-      <c r="G26" s="9" t="n">
+      <c r="G26" s="1" t="n">
         <f aca="false">G7-G18</f>
         <v>-0.01</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C27" s="2" t="n">
         <v>203</v>
       </c>
-      <c r="D27" s="9" t="n">
+      <c r="D27" s="1" t="n">
         <f aca="false">D8-D19</f>
         <v>-0.07</v>
       </c>
-      <c r="E27" s="9" t="n">
+      <c r="E27" s="1" t="n">
         <f aca="false">E8-E19</f>
         <v>-0.01</v>
       </c>
-      <c r="F27" s="9" t="n">
+      <c r="F27" s="1" t="n">
         <f aca="false">F8-F19</f>
         <v>0</v>
       </c>
-      <c r="G27" s="9" t="n">
+      <c r="G27" s="1" t="n">
         <f aca="false">G8-G19</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C28" s="2" t="n">
         <v>215</v>
       </c>
-      <c r="D28" s="9" t="n">
+      <c r="D28" s="1" t="n">
         <f aca="false">D9-D20</f>
         <v>-0.13</v>
       </c>
-      <c r="E28" s="9" t="n">
+      <c r="E28" s="1" t="n">
         <f aca="false">E9-E20</f>
         <v>0</v>
       </c>
-      <c r="F28" s="9" t="n">
+      <c r="F28" s="1" t="n">
         <f aca="false">F9-F20</f>
         <v>0</v>
       </c>
-      <c r="G28" s="9" t="n">
+      <c r="G28" s="1" t="n">
         <f aca="false">G9-G20</f>
         <v>-0.11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C29" s="2" t="n">
         <v>254</v>
       </c>
-      <c r="D29" s="9" t="n">
+      <c r="D29" s="1" t="n">
         <f aca="false">D10-D21</f>
         <v>0</v>
       </c>
-      <c r="E29" s="9" t="n">
+      <c r="E29" s="1" t="n">
         <f aca="false">E10-E21</f>
         <v>-0.02</v>
       </c>
-      <c r="F29" s="9" t="n">
+      <c r="F29" s="1" t="n">
         <f aca="false">F10-F21</f>
         <v>-0.03</v>
       </c>
-      <c r="G29" s="9" t="n">
+      <c r="G29" s="1" t="n">
         <f aca="false">G10-G21</f>
         <v>-0.01</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1897,98 +1822,98 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.92"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.5</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>606035</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>178</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.13</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>600540</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.24</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>203</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0.05</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>676079</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.45</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>215</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.26</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>606017</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>0.16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>254</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>0.06</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the original Excel file for comparison with the one we write the solutions to.
</commit_message>
<xml_diff>
--- a/exercise-6/Produkt_miks.xlsx
+++ b/exercise-6/Produkt_miks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basismodell" sheetId="1" state="visible" r:id="rId2"/>
@@ -560,11 +560,11 @@
   </sheetPr>
   <dimension ref="B1:K30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.03"/>
@@ -810,11 +810,11 @@
   </sheetPr>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.78"/>
@@ -1008,10 +1008,10 @@
   <dimension ref="A1:AA44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R36" activeCellId="0" sqref="R36"/>
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.28"/>
@@ -1822,7 +1822,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.92"/>

</xml_diff>

<commit_message>
Løsning for problem 2 lagt til.
</commit_message>
<xml_diff>
--- a/exercise-6/Produkt_miks.xlsx
+++ b/exercise-6/Produkt_miks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Basismodell" sheetId="1" state="visible" r:id="rId2"/>
@@ -364,7 +364,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,6 +399,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFE2F0D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF5983B0"/>
       </patternFill>
     </fill>
   </fills>
@@ -436,7 +442,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -470,6 +476,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -508,7 +518,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFF2CC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -564,7 +574,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.03"/>
@@ -810,11 +820,11 @@
   </sheetPr>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.78"/>
@@ -857,16 +867,16 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="9" t="n">
         <v>0.15</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="9" t="n">
         <v>0.24</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="9" t="n">
         <v>0.45</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="9" t="n">
         <v>0.16</v>
       </c>
     </row>
@@ -875,15 +885,24 @@
       <c r="B5" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="9" t="n">
         <v>0.5</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="n">
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6" t="n">
         <f aca="false">SUM(D5:G5)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -891,78 +910,114 @@
       <c r="B6" s="2" t="n">
         <v>178</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="9" t="n">
         <v>0.13</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="n">
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6" t="n">
         <f aca="false">SUM(D6:G6)</f>
-        <v>0</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="n">
         <v>203</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="9" t="n">
         <v>0.05</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1" t="n">
+      <c r="D7" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6" t="n">
         <f aca="false">SUM(D7:G7)</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
         <v>215</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="9" t="n">
         <v>0.26</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1" t="n">
+      <c r="D8" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="H8" s="6" t="n">
         <f aca="false">SUM(D8:G8)</f>
-        <v>0</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="n">
         <v>254</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="9" t="n">
         <v>0.06</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="n">
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>0.0600000000000001</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6" t="n">
         <f aca="false">SUM(D9:G9)</f>
-        <v>0</v>
+        <v>0.0600000000000001</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="6" t="n">
         <f aca="false">SUM(D5:D9)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="E10" s="6" t="n">
         <f aca="false">SUM(E5:E9)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="1" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="F10" s="6" t="n">
         <f aca="false">SUM(F5:F9)</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="1" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="G10" s="6" t="n">
         <f aca="false">SUM(G5:G9)</f>
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -1007,11 +1062,11 @@
   </sheetPr>
   <dimension ref="A1:AA44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.28"/>
@@ -1275,7 +1330,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="2" t="n">
@@ -1293,7 +1348,7 @@
       <c r="G17" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="I17" s="10" t="n">
+      <c r="I17" s="11" t="n">
         <f aca="false">SUM(D17:G21)</f>
         <v>0.9985</v>
       </c>
@@ -1822,7 +1877,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.92"/>

</xml_diff>

<commit_message>
Added writing to file for the threshold model.
</commit_message>
<xml_diff>
--- a/exercise-6/Produkt_miks.xlsx
+++ b/exercise-6/Produkt_miks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basismodell" sheetId="1" state="visible" r:id="rId2"/>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
   <si>
     <t xml:space="preserve">Løst i Python:</t>
   </si>
@@ -275,6 +275,12 @@
   </si>
   <si>
     <t xml:space="preserve">Beregnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingen begrensninger på ulovlige kombinasjoner av diametere og legeringer:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum andel:</t>
   </si>
   <si>
     <t xml:space="preserve">Positivt avvik</t>
@@ -364,7 +370,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +413,12 @@
         <bgColor rgb="FF5983B0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB66C"/>
+        <bgColor rgb="FFFF99CC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
@@ -442,7 +454,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -480,6 +492,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -541,7 +561,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFB66C"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -574,7 +594,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.03"/>
@@ -818,13 +838,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.78"/>
@@ -1044,7 +1064,204 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D22" s="2" t="n">
+        <v>606035</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>600540</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>676079</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>606017</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="9" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="E23" s="9" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="F23" s="9" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="G23" s="9" t="n">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="C24" s="9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6" t="n">
+        <f aca="false">SUM(D24:G24)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="2" t="n">
+        <v>178</v>
+      </c>
+      <c r="C25" s="9" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H25" s="6" t="n">
+        <f aca="false">SUM(D25:G25)</f>
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="2" t="n">
+        <v>203</v>
+      </c>
+      <c r="C26" s="9" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H26" s="6" t="n">
+        <f aca="false">SUM(D26:G26)</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="2" t="n">
+        <v>215</v>
+      </c>
+      <c r="C27" s="9" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="6" t="n">
+        <f aca="false">SUM(D27:G27)</f>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="2" t="n">
+        <v>254</v>
+      </c>
+      <c r="C28" s="9" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="H28" s="6" t="n">
+        <f aca="false">SUM(D28:G28)</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D29" s="6" t="n">
+        <f aca="false">SUM(D24:D28)</f>
+        <v>0.15</v>
+      </c>
+      <c r="E29" s="6" t="n">
+        <f aca="false">SUM(E24:E28)</f>
+        <v>0.24</v>
+      </c>
+      <c r="F29" s="6" t="n">
+        <f aca="false">SUM(F24:F28)</f>
+        <v>0.45</v>
+      </c>
+      <c r="G29" s="6" t="n">
+        <f aca="false">SUM(G24:G28)</f>
+        <v>0.16</v>
+      </c>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C19:H19"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1062,11 +1279,11 @@
   </sheetPr>
   <dimension ref="A1:AA44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.28"/>
@@ -1228,22 +1445,22 @@
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="L13" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1263,7 +1480,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
@@ -1281,7 +1498,7 @@
         <v>606017</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>3</v>
@@ -1330,8 +1547,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>15</v>
+      <c r="A17" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>152</v>
@@ -1348,7 +1565,7 @@
       <c r="G17" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="I17" s="11" t="n">
+      <c r="I17" s="13" t="n">
         <f aca="false">SUM(D17:G21)</f>
         <v>0.9985</v>
       </c>
@@ -1714,7 +1931,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
@@ -1734,7 +1951,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>152</v>
@@ -1877,7 +2094,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.92"/>
@@ -1888,13 +2105,13 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>